<commit_message>
feat: add store and warehouse stock in inventory stock report
</commit_message>
<xml_diff>
--- a/api/utils/templates/xlsx/baseInventory.xlsx
+++ b/api/utils/templates/xlsx/baseInventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugod\Desktop\proyectos\maximport\sources\max-import-backend\api\utils\templates\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3276C03E-A81A-4B77-BC95-662AB8C72BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348CF137-E4E1-4792-A578-38DF5527B62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="3375" windowWidth="21600" windowHeight="11295" xr2:uid="{3F90E08B-5E6B-4E95-9F51-698F115049C6}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="12975" xr2:uid="{3F90E08B-5E6B-4E95-9F51-698F115049C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>LISTA DE  DE INVENTARIO</t>
   </si>
@@ -57,10 +57,13 @@
     <t>NOMBRE</t>
   </si>
   <si>
-    <t>STOCK</t>
-  </si>
-  <si>
     <t>CAJAS</t>
+  </si>
+  <si>
+    <t>EN TIENDA</t>
+  </si>
+  <si>
+    <t>EN ALMACEN</t>
   </si>
 </sst>
 </file>
@@ -110,11 +113,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -430,64 +438,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF94AF20-A2FF-4736-94BE-B00DDB288A13}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.86328125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="17.3984375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>